<commit_message>
Correção a use cases e modelação da interface
</commit_message>
<xml_diff>
--- a/Parte2/use_cases/Apresenta informação extra de ação.xlsx
+++ b/Parte2/use_cases/Apresenta informação extra de ação.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelarodrigues/Desktop/Trabalhos/Dolce_Cheferini/Parte2/use_cases/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\LI4\Parte2\use_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34B9346-298D-F844-ADB7-CBB7A1462128}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC4B181-BF51-4FEB-85E2-D810BF88BC2A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Use Case:</t>
   </si>
@@ -74,6 +74,12 @@
   </si>
   <si>
     <t>1.2 Impede execução de receita</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alternativa 2 [requisita repetição de esclarecimento] (Passo 1)</t>
+  </si>
+  <si>
+    <t>1.1 Regressa a 1</t>
   </si>
 </sst>
 </file>
@@ -293,14 +299,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,59 +690,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D14"/>
+  <dimension ref="B2:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.625" customWidth="1"/>
     <col min="3" max="3" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="72.1640625" customWidth="1"/>
+    <col min="4" max="4" width="72.125" customWidth="1"/>
     <col min="5" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="D2" s="12"/>
+    </row>
+    <row r="3" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="2:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="D4" s="12"/>
+    </row>
+    <row r="5" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
+      <c r="D5" s="13"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -746,32 +752,32 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="12"/>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="14"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="14"/>
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
+    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="14"/>
       <c r="C9" s="6"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="12"/>
+    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="14"/>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="2:4" ht="21" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="9"/>
@@ -779,31 +785,56 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="12"/>
+    <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="14"/>
       <c r="C12" s="6"/>
       <c r="D12" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
+    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="14"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="2:4" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="12"/>
+    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="14"/>
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
     </row>
+    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="14"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="11"/>
+    </row>
+    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="14"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="14"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B15:B18"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B6:B10"/>
-    <mergeCell ref="B11:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Correção ao Diagrama Lógico e Use case de Ementa Semanal
</commit_message>
<xml_diff>
--- a/Parte2/use_cases/Apresenta informação extra de ação.xlsx
+++ b/Parte2/use_cases/Apresenta informação extra de ação.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\LI4\Parte2\use_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC4B181-BF51-4FEB-85E2-D810BF88BC2A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD805EA6-424B-4BBC-A478-A62592B1E039}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -299,14 +299,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,10 +690,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D18"/>
+  <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -709,40 +709,40 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="12"/>
+      <c r="D2" s="13"/>
     </row>
     <row r="3" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="12"/>
+      <c r="D3" s="13"/>
     </row>
     <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="14"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -753,88 +753,83 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="14"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="14"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="14"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="14"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="8"/>
+      <c r="B10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="9"/>
+      <c r="D10" s="10" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="D11" s="10" t="s">
-        <v>14</v>
+      <c r="B11" s="12"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="11" t="s">
-        <v>15</v>
-      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="10" t="s">
-        <v>17</v>
-      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="11"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="14"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="14"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="14"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="8"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="B6:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Mais update a diagramas
</commit_message>
<xml_diff>
--- a/Parte2/use_cases/Apresenta informação extra de ação.xlsx
+++ b/Parte2/use_cases/Apresenta informação extra de ação.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\LI4\Parte2\use_cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD805EA6-424B-4BBC-A478-A62592B1E039}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F34F9938-3701-4ECE-8EFC-261D7F405492}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="3240" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>Actor:</t>
   </si>
   <si>
-    <t>Utilizador</t>
-  </si>
-  <si>
     <t>Pré condição:</t>
   </si>
   <si>
@@ -52,12 +49,6 @@
     <t>System response</t>
   </si>
   <si>
-    <t>Apresenta informação extra de ação</t>
-  </si>
-  <si>
-    <t>Ação selecionada</t>
-  </si>
-  <si>
     <t>Informação extra visualizada</t>
   </si>
   <si>
@@ -80,6 +71,15 @@
   </si>
   <si>
     <t>1.1 Regressa a 1</t>
+  </si>
+  <si>
+    <t>Apresenta informação extra</t>
+  </si>
+  <si>
+    <t>Utilizador autenticado</t>
+  </si>
+  <si>
+    <t>A confecionar passo</t>
   </si>
 </sst>
 </file>
@@ -95,11 +95,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -281,17 +280,23 @@
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -299,14 +304,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -690,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D17"/>
+  <dimension ref="B2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -705,131 +704,126 @@
     <col min="5" max="1025" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="13"/>
-    </row>
-    <row r="3" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="13"/>
-    </row>
-    <row r="4" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="4"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="4"/>
+      <c r="C8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="14" t="s">
+      <c r="D8" s="10"/>
+    </row>
+    <row r="9" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="12"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="12"/>
-      <c r="C8" s="6" t="s">
+    <row r="10" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="12"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="12" t="s">
+    </row>
+    <row r="11" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="10" t="s">
+      <c r="C13" s="11"/>
+      <c r="D13" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="12"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="12"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="12"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="D14" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="12"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="11"/>
-    </row>
-    <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="12"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="12"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
+    <row r="14" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="4"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="B13:B16"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B6:B8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>